<commit_message>
Update info clase 04 File System
</commit_message>
<xml_diff>
--- a/00-indice-videos.xlsx
+++ b/00-indice-videos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caryces\Desktop\CENDEZ\Formacion Academica\Programacion\Programacion Autonomo\coderhouse\04-Backend\01-info\Programación Backend I Desarrollo Avanzado de Backend\_00-videos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caryces\Desktop\CENDEZ\Formacion Academica\Programacion\Programacion Autonomo\coderhouse\04-Backend\01-info\Backend-I\_00-videos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A8F33F-DE07-4A32-8B90-6235E6015A21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{135755A5-CA6B-4FA0-BDD5-24A15410E708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43200" yWindow="0" windowWidth="14400" windowHeight="15750" xr2:uid="{5152FF14-2E32-4855-8483-EEC7775E3DF9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Clase 00</t>
   </si>
@@ -168,6 +168,66 @@
   </si>
   <si>
     <t>Ejemplo con API de GitHub</t>
+  </si>
+  <si>
+    <t>Clase 04</t>
+  </si>
+  <si>
+    <t>Que es Node JS</t>
+  </si>
+  <si>
+    <t>Actividad en clase: Proyecto de node (generar 10000 numeros aleatorios de 1 a 20)</t>
+  </si>
+  <si>
+    <t>Uso de metodo Math</t>
+  </si>
+  <si>
+    <t>Modulos nativos de Nodejs</t>
+  </si>
+  <si>
+    <t>Observacion en cambio del orden de las clase, primero fs despues crypto</t>
+  </si>
+  <si>
+    <t>Ejemplo de setTimeout</t>
+  </si>
+  <si>
+    <t>Ejemplo de setTimeinterval</t>
+  </si>
+  <si>
+    <t>Manejo de archivos - La persistencia en memoria</t>
+  </si>
+  <si>
+    <t>file system en NodeJs</t>
+  </si>
+  <si>
+    <t>metodo writeFileSync()</t>
+  </si>
+  <si>
+    <t>metodo appendFileSync()</t>
+  </si>
+  <si>
+    <t>metodo existsSync()</t>
+  </si>
+  <si>
+    <t>metodo readFile()</t>
+  </si>
+  <si>
+    <t>File System de manera Asincronica (promises) - no tienen --Sync-- al final</t>
+  </si>
+  <si>
+    <t>metodo appendFile()</t>
+  </si>
+  <si>
+    <t>archivos .json</t>
+  </si>
+  <si>
+    <t xml:space="preserve">metodo JSON.stringify() - para pasar de tipo objeto JS a texto plano de tipo JSON </t>
+  </si>
+  <si>
+    <t>metodo JSON.parse() - para pasar de texto plano de tipo JSON  a tipo objeto JS</t>
+  </si>
+  <si>
+    <t>Hands on Labs - "Manager de usuarios"</t>
   </si>
 </sst>
 </file>
@@ -580,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8F680E1-5CBF-4782-AF11-5D549B1A7385}">
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:B64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -937,6 +997,164 @@
         <v>43</v>
       </c>
     </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" s="2"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="4">
+        <v>3.1250000000000002E-3</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="4">
+        <v>4.8611111111111112E-3</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="4">
+        <v>8.6805555555555559E-3</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="4">
+        <v>1.9791666666666666E-2</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="4">
+        <v>2.1180555555555557E-2</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="4">
+        <v>2.8819444444444446E-2</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="4">
+        <v>3.0902777777777779E-2</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="4">
+        <v>3.1944444444444442E-2</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="4">
+        <v>3.4027777777777775E-2</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="4">
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="4">
+        <v>3.8194444444444448E-2</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="4">
+        <v>3.888888888888889E-2</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="4">
+        <v>4.3402777777777776E-2</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="4">
+        <v>4.4444444444444446E-2</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="4">
+        <v>4.5486111111111109E-2</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="4">
+        <v>5.1736111111111108E-2</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="4">
+        <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="4">
+        <v>5.3124999999999999E-2</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="4">
+        <v>6.145833333333333E-2</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B21" r:id="rId1" xr:uid="{921E25A7-FC31-4CD8-810B-6AB13253BAF7}"/>

</xml_diff>

<commit_message>
actualizacion hasta clase NPM dependencias
</commit_message>
<xml_diff>
--- a/00-indice-videos.xlsx
+++ b/00-indice-videos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caryces\Desktop\CENDEZ\Formacion Academica\Programacion\Programacion Autonomo\coderhouse\04-Backend\01-info\Backend-I\_00-videos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{135755A5-CA6B-4FA0-BDD5-24A15410E708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED1ADB8-BC4E-472C-B757-6C3ACC5BE78E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43200" yWindow="0" windowWidth="14400" windowHeight="15750" xr2:uid="{5152FF14-2E32-4855-8483-EEC7775E3DF9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
   <si>
     <t>Clase 00</t>
   </si>
@@ -228,6 +228,84 @@
   </si>
   <si>
     <t>Hands on Labs - "Manager de usuarios"</t>
+  </si>
+  <si>
+    <t>Clase 05</t>
+  </si>
+  <si>
+    <t>Hands on lab "Crypto" - Creacion de clase "UsersManager"</t>
+  </si>
+  <si>
+    <t>Explica que el uso asyncrono en este ejemplo es para familiarizarse al momento de uso en base de datos</t>
+  </si>
+  <si>
+    <t>llamar a un metodo dentro de la clase usando this ej: this.getUsers()</t>
+  </si>
+  <si>
+    <t>https://nodejs.org/api/crypto.html</t>
+  </si>
+  <si>
+    <t>metodo crypto.createHmac()</t>
+  </si>
+  <si>
+    <t>metodo crypto.randomBytes() (es como si fuese un Math.random pero para crypto)</t>
+  </si>
+  <si>
+    <t>metodos .update()  y .digest()</t>
+  </si>
+  <si>
+    <t>createUser()</t>
+  </si>
+  <si>
+    <t>validateUser() - username y password para login</t>
+  </si>
+  <si>
+    <t>Modulos de terceros - ¿Qué es NPM?</t>
+  </si>
+  <si>
+    <t>https://npmjs.com</t>
+  </si>
+  <si>
+    <t>Ejemplo Creacion proyecto NPM</t>
+  </si>
+  <si>
+    <t>Instalacion de una dependencia o librería</t>
+  </si>
+  <si>
+    <t>.gitignore</t>
+  </si>
+  <si>
+    <t>devDependencies - nodemon (para que sirve)</t>
+  </si>
+  <si>
+    <t>script start</t>
+  </si>
+  <si>
+    <t>dependencia uuid sirve para generar id aleatorio</t>
+  </si>
+  <si>
+    <t>dependencias globales y locales - (global se instala con  -g)</t>
+  </si>
+  <si>
+    <t>node version 18 tiene utilidad --watch que reemplaza nodemon.</t>
+  </si>
+  <si>
+    <t>Simbolo "&gt;" en el numero de version. Instala la ultima version. --no recomendado--</t>
+  </si>
+  <si>
+    <t>Simbolo "~" en el numero de version. Instala la ultima version del patch (tercer numero)</t>
+  </si>
+  <si>
+    <t>Versionado de dependencias (instalacion por versiones). Que significan los numeros en las versiones ej: 9.0.1</t>
+  </si>
+  <si>
+    <t>Desinstalar una version e instalar una version diferente</t>
+  </si>
+  <si>
+    <t>npm outdated - para saber que actualizacione tengo disponibles para las dependencias</t>
+  </si>
+  <si>
+    <t>Simbolo "^" en el numero de version. Instala la ultima actualizacion de esa version mayor --recomendado--</t>
   </si>
 </sst>
 </file>
@@ -640,10 +718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8F680E1-5CBF-4782-AF11-5D549B1A7385}">
-  <dimension ref="A1:B64"/>
+  <dimension ref="A1:B90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1155,9 +1233,217 @@
         <v>63</v>
       </c>
     </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B65" s="2"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="4">
+        <v>4.5138888888888885E-3</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="4">
+        <v>1.1111111111111112E-2</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="4">
+        <v>1.5277777777777777E-2</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="4">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A70" s="4">
+        <v>1.7013888888888887E-2</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="4">
+        <v>2.013888888888889E-2</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="4">
+        <v>2.1180555555555557E-2</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="4">
+        <v>2.2916666666666665E-2</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" s="4">
+        <v>3.0208333333333334E-2</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="4">
+        <v>4.7569444444444442E-2</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A76" s="4">
+        <v>4.8263888888888891E-2</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="4">
+        <v>4.9652777777777775E-2</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="4">
+        <v>5.1388888888888887E-2</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="4">
+        <v>5.3124999999999999E-2</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="4">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="4">
+        <v>5.6250000000000001E-2</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="4">
+        <v>5.8333333333333334E-2</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="4">
+        <v>6.0069444444444446E-2</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="4">
+        <v>6.2152777777777779E-2</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="4">
+        <v>6.3194444444444442E-2</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="4">
+        <v>6.5972222222222224E-2</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="4">
+        <v>6.7013888888888887E-2</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="4">
+        <v>6.8402777777777785E-2</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="4">
+        <v>6.9097222222222227E-2</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="4">
+        <v>7.1874999999999994E-2</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B21" r:id="rId1" xr:uid="{921E25A7-FC31-4CD8-810B-6AB13253BAF7}"/>
+    <hyperlink ref="B70" r:id="rId2" xr:uid="{9A04AE78-5D84-4392-B67B-0690FED34630}"/>
+    <hyperlink ref="B76" r:id="rId3" xr:uid="{F5276926-B70F-40D8-A4F2-BA2A8B85CDB4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualizacion hasta clase 06 Servidores
</commit_message>
<xml_diff>
--- a/00-indice-videos.xlsx
+++ b/00-indice-videos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caryces\Desktop\CENDEZ\Formacion Academica\Programacion\Programacion Autonomo\coderhouse\04-Backend\01-info\Backend-I\_00-videos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED1ADB8-BC4E-472C-B757-6C3ACC5BE78E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{834CC086-41A4-4CC0-A60B-72EB92086778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43200" yWindow="0" windowWidth="14400" windowHeight="15750" xr2:uid="{5152FF14-2E32-4855-8483-EEC7775E3DF9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
   <si>
     <t>Clase 00</t>
   </si>
@@ -306,6 +306,72 @@
   </si>
   <si>
     <t>Simbolo "^" en el numero de version. Instala la ultima actualizacion de esa version mayor --recomendado--</t>
+  </si>
+  <si>
+    <t>Clase 06</t>
+  </si>
+  <si>
+    <t>Protocolo HTTP</t>
+  </si>
+  <si>
+    <t>cliente =&gt; request  // servidor =&gt; responses   ( Frontend // Backend )</t>
+  </si>
+  <si>
+    <t>Instalar nodemon de manera global (ver fila 84)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Propiedad "type": "module" para activar import y export </t>
+  </si>
+  <si>
+    <t>script "dev": "nodemon server-http .js"</t>
+  </si>
+  <si>
+    <t>request (Propiedades, solicitado por el cliente) y response en el createServer</t>
+  </si>
+  <si>
+    <t>res.end enviar informacion al cliente</t>
+  </si>
+  <si>
+    <t>Thunder Client (Cliente https)</t>
+  </si>
+  <si>
+    <t>Postman, el que se usara en clase</t>
+  </si>
+  <si>
+    <t>Endpoints</t>
+  </si>
+  <si>
+    <t>Creacion de un Endpoint</t>
+  </si>
+  <si>
+    <t>Objeto Request  ( req )</t>
+  </si>
+  <si>
+    <t>https://expressjs.com</t>
+  </si>
+  <si>
+    <t>Express  -  npm i express</t>
+  </si>
+  <si>
+    <t>Express aplica el tipo de archivo sin usar el stringify, devuelve los datos en formato JSON</t>
+  </si>
+  <si>
+    <t>Desde el servidor somos los responsables de crear los estatus, errores del servidor</t>
+  </si>
+  <si>
+    <t>Propiedad req.query</t>
+  </si>
+  <si>
+    <t>Propiedad req.params</t>
+  </si>
+  <si>
+    <t>Metodo get</t>
+  </si>
+  <si>
+    <t>Metodo post</t>
+  </si>
+  <si>
+    <t>Middleware para procesar JSON en el cuerpo de las solicitudes POST  app.use(express.json());</t>
   </si>
 </sst>
 </file>
@@ -718,10 +784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8F680E1-5CBF-4782-AF11-5D549B1A7385}">
-  <dimension ref="A1:B90"/>
+  <dimension ref="A1:B112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="B87" sqref="B87"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="A113" sqref="A113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1439,11 +1505,186 @@
         <v>88</v>
       </c>
     </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B91" s="2"/>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="4">
+        <v>3.1250000000000002E-3</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="4">
+        <v>9.7222222222222224E-3</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" s="4">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="4">
+        <v>1.6319444444444445E-2</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" s="4">
+        <v>1.9097222222222224E-2</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" s="4">
+        <v>2.1527777777777778E-2</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="4">
+        <v>2.326388888888889E-2</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" s="4">
+        <v>2.4305555555555556E-2</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" s="4">
+        <v>2.5347222222222222E-2</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" s="4">
+        <v>2.8125000000000001E-2</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" s="4">
+        <v>3.0555555555555555E-2</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" s="4">
+        <v>3.6805555555555557E-2</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" s="4">
+        <v>4.3749999999999997E-2</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A105" s="4">
+        <v>4.4444444444444446E-2</v>
+      </c>
+      <c r="B105" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" s="4">
+        <v>4.7222222222222221E-2</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" s="4">
+        <v>5.0347222222222224E-2</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" s="4">
+        <v>5.1388888888888887E-2</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" s="4">
+        <v>6.0069444444444446E-2</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" s="4">
+        <v>7.1874999999999994E-2</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" s="4">
+        <v>7.7083333333333337E-2</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" s="4">
+        <v>7.9166666666666663E-2</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B21" r:id="rId1" xr:uid="{921E25A7-FC31-4CD8-810B-6AB13253BAF7}"/>
     <hyperlink ref="B70" r:id="rId2" xr:uid="{9A04AE78-5D84-4392-B67B-0690FED34630}"/>
     <hyperlink ref="B76" r:id="rId3" xr:uid="{F5276926-B70F-40D8-A4F2-BA2A8B85CDB4}"/>
+    <hyperlink ref="B105" r:id="rId4" xr:uid="{A4759B5C-9A6B-4C65-9E6B-78706D6197B9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Clases 07 y 08
</commit_message>
<xml_diff>
--- a/00-indice-videos.xlsx
+++ b/00-indice-videos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caryces\Desktop\CENDEZ\Formacion Academica\Programacion\Programacion Autonomo\coderhouse\04-Backend\01-info\Backend-I\_00-videos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{834CC086-41A4-4CC0-A60B-72EB92086778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397B4F1E-F8E0-4050-BB29-CC27AD5DAC5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43200" yWindow="0" windowWidth="14400" windowHeight="15750" xr2:uid="{5152FF14-2E32-4855-8483-EEC7775E3DF9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="151">
   <si>
     <t>Clase 00</t>
   </si>
@@ -372,6 +372,123 @@
   </si>
   <si>
     <t>Middleware para procesar JSON en el cuerpo de las solicitudes POST  app.use(express.json());</t>
+  </si>
+  <si>
+    <t>Clase 07</t>
+  </si>
+  <si>
+    <t>Codigos de estado (1xx, 2xx, 3xx, 4xx, 5xx)</t>
+  </si>
+  <si>
+    <t>Lo ideal es agregar un codigo de estado en la respuesta. Para que express no lo haga por defecto</t>
+  </si>
+  <si>
+    <t>Formatos JSON y XML (Este ultimo casi no se utiliza en la actualidad)</t>
+  </si>
+  <si>
+    <t>API REST</t>
+  </si>
+  <si>
+    <t>Modelo de una API REST</t>
+  </si>
+  <si>
+    <t>Metodos de peticion</t>
+  </si>
+  <si>
+    <t>Copiando el user.manager con los metodos getUsers y createUser</t>
+  </si>
+  <si>
+    <t>importar uuid</t>
+  </si>
+  <si>
+    <t>modificacion createUser</t>
+  </si>
+  <si>
+    <t>creacion de getUserById</t>
+  </si>
+  <si>
+    <t>creacion de updateUser</t>
+  </si>
+  <si>
+    <t>creacion de deleteUser</t>
+  </si>
+  <si>
+    <t>Middleware para datos que se envian por parametros, por URL</t>
+  </si>
+  <si>
+    <t>Endpoint app.get('/users'</t>
+  </si>
+  <si>
+    <t>Endpoint app.get('/users/:id'</t>
+  </si>
+  <si>
+    <t>Endpoint app.post('/users'</t>
+  </si>
+  <si>
+    <t>Explicacion postman</t>
+  </si>
+  <si>
+    <t>Endpoint app.put('</t>
+  </si>
+  <si>
+    <t>Endpoint app.delete('</t>
+  </si>
+  <si>
+    <t>Clase 08</t>
+  </si>
+  <si>
+    <t>Router en Express</t>
+  </si>
+  <si>
+    <t>Pasando las Rutas del server.js al user.router.js</t>
+  </si>
+  <si>
+    <t>Revisando con postman despues de los cambios</t>
+  </si>
+  <si>
+    <t>concepto modularizacion</t>
+  </si>
+  <si>
+    <t>Hands on lab "Users y Pets"</t>
+  </si>
+  <si>
+    <t>Cada Router deberia tener su propio manager. El ejemplo de Pets se hizo asi solo por explicacion</t>
+  </si>
+  <si>
+    <t>Middleware static  app.use(express.static('public'))</t>
+  </si>
+  <si>
+    <t>Hay Middlewares a nivel de aplicación, a nivel de enrutador y a nivel de endpoint</t>
+  </si>
+  <si>
+    <t>Ejemplo de como funciona un Middleware</t>
+  </si>
+  <si>
+    <t>__dirname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Archivos estaticos con express.static (imagen, html) </t>
+  </si>
+  <si>
+    <t>definicion ¿Qué es un middleware?</t>
+  </si>
+  <si>
+    <t>Multer es un Middleware que permite subir archivos al servidor</t>
+  </si>
+  <si>
+    <t>Tipos de Middleware</t>
+  </si>
+  <si>
+    <t>Multer - Es un middleware de terceros</t>
+  </si>
+  <si>
+    <t>Instalacion de multer</t>
+  </si>
+  <si>
+    <t>Archivo multer.js</t>
+  </si>
+  <si>
+    <t>Subiendo una imagen como adjunto con postman</t>
   </si>
 </sst>
 </file>
@@ -784,10 +901,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8F680E1-5CBF-4782-AF11-5D549B1A7385}">
-  <dimension ref="A1:B112"/>
+  <dimension ref="A1:B152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A113" sqref="A113"/>
+    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
+      <selection activeCell="B152" sqref="B152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1679,6 +1796,322 @@
         <v>111</v>
       </c>
     </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B113" s="2"/>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" s="4">
+        <v>2.7777777777777779E-3</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" s="4">
+        <v>4.8611111111111112E-3</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" s="4">
+        <v>7.2916666666666668E-3</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" s="4">
+        <v>1.0069444444444445E-2</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" s="4">
+        <v>1.1111111111111112E-2</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" s="4">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" s="4">
+        <v>1.4930555555555556E-2</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" s="4">
+        <v>1.6319444444444445E-2</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" s="4">
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" s="4">
+        <v>2.013888888888889E-2</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" s="4">
+        <v>2.1874999999999999E-2</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" s="4">
+        <v>2.5347222222222222E-2</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" s="4">
+        <v>2.7430555555555555E-2</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" s="4">
+        <v>2.8125000000000001E-2</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" s="4">
+        <v>3.0555555555555555E-2</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" s="4">
+        <v>3.6111111111111108E-2</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" s="4">
+        <v>4.4791666666666667E-2</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" s="4">
+        <v>5.7291666666666664E-2</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" s="4">
+        <v>6.1805555555555558E-2</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B133" s="2"/>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134" s="4">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" s="4">
+        <v>5.9027777777777776E-3</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" s="4">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137" s="4">
+        <v>1.2847222222222222E-2</v>
+      </c>
+      <c r="B137" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" s="4">
+        <v>1.3541666666666667E-2</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" s="4">
+        <v>2.013888888888889E-2</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" s="4">
+        <v>2.0486111111111111E-2</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" s="4">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="B141" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142" s="4">
+        <v>2.1527777777777778E-2</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143" s="4">
+        <v>2.2916666666666665E-2</v>
+      </c>
+      <c r="B143" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144" s="4">
+        <v>3.125E-2</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" s="4">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="B145" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" s="4">
+        <v>4.9652777777777775E-2</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147" s="4">
+        <v>5.1388888888888887E-2</v>
+      </c>
+      <c r="B147" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148" s="4">
+        <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="B148" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149" s="4">
+        <v>5.3124999999999999E-2</v>
+      </c>
+      <c r="B149" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150" s="4">
+        <v>5.4166666666666669E-2</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151" s="4">
+        <v>5.5208333333333331E-2</v>
+      </c>
+      <c r="B151" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152" s="4">
+        <v>6.2847222222222221E-2</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B21" r:id="rId1" xr:uid="{921E25A7-FC31-4CD8-810B-6AB13253BAF7}"/>

</xml_diff>

<commit_message>
hasta clase 14 mongoose
</commit_message>
<xml_diff>
--- a/00-indice-videos.xlsx
+++ b/00-indice-videos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caryces\Desktop\CENDEZ\Formacion Academica\Programacion\Programacion Autonomo\coderhouse\04-Backend\01-info\Backend-I\_00-videos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56FAB917-4DCB-4DB5-8DC8-1A8A06F520B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{157B7D57-374B-4503-A8AB-1C3902416355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43200" yWindow="0" windowWidth="14400" windowHeight="15750" xr2:uid="{5152FF14-2E32-4855-8483-EEC7775E3DF9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="327">
   <si>
     <t>Clase 00</t>
   </si>
@@ -939,6 +939,84 @@
   </si>
   <si>
     <t>Mongoose</t>
+  </si>
+  <si>
+    <t>Clientes de BD</t>
+  </si>
+  <si>
+    <t>Cliente GUI (Mongo Compass)</t>
+  </si>
+  <si>
+    <t>Cliente App (desde node ==&gt; Mongoose)  // Cliente Web ==&gt;  Mongo atlas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ODM ==&gt; mongoose, es un traductor entre el codigo y la base de datos </t>
+  </si>
+  <si>
+    <t>DBaaS (Database as a Service) Mongo Altlas</t>
+  </si>
+  <si>
+    <t>Explicacion de modelos en la nube como servicio (Cloud Models)</t>
+  </si>
+  <si>
+    <t>Mongo Atlas</t>
+  </si>
+  <si>
+    <t>Configuracion de Mongo Atlas</t>
+  </si>
+  <si>
+    <t>Panel de Mongo Atlas</t>
+  </si>
+  <si>
+    <t>Configuracion Network Access IP</t>
+  </si>
+  <si>
+    <t>Configuracion de usuario</t>
+  </si>
+  <si>
+    <t>Conexion a base de datos</t>
+  </si>
+  <si>
+    <t>Conexión con MongoDB Compass</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Conexión de cero, instalacion mongoose</t>
+  </si>
+  <si>
+    <t>Mongoose ==&gt; sirve para definir esquemas definidos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">donde poner el nombre de la "base de datos" en la url de conexión  </t>
+  </si>
+  <si>
+    <t>function de conexión a la base de datos</t>
+  </si>
+  <si>
+    <t>Creacion del Schema</t>
+  </si>
+  <si>
+    <t>Archivo registro.js</t>
+  </si>
+  <si>
+    <t>Metodos en CRUD en el product manager</t>
+  </si>
+  <si>
+    <t>Controllers</t>
+  </si>
+  <si>
+    <t>del manager se pasa al controller</t>
+  </si>
+  <si>
+    <t>repaso de las carpetas y archivos generados</t>
+  </si>
+  <si>
+    <t>Clase 15</t>
+  </si>
+  <si>
+    <t>Primera práctica integradora</t>
   </si>
 </sst>
 </file>
@@ -1351,16 +1429,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8F680E1-5CBF-4782-AF11-5D549B1A7385}">
-  <dimension ref="A1:B288"/>
+  <dimension ref="A1:C312"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A259" workbookViewId="0">
-      <selection activeCell="B289" sqref="B289"/>
+    <sheetView tabSelected="1" topLeftCell="A280" workbookViewId="0">
+      <selection activeCell="A313" sqref="A313"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="106.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="115.7109375" style="2" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -3666,6 +3744,201 @@
       </c>
       <c r="B288" s="1" t="s">
         <v>300</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A289" s="3">
+        <v>2.4305555555555556E-3</v>
+      </c>
+      <c r="B289" s="2" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A290" s="3">
+        <v>3.1250000000000002E-3</v>
+      </c>
+      <c r="B290" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A291" s="3">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="B291" s="2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A292" s="3">
+        <v>4.8611111111111112E-3</v>
+      </c>
+      <c r="B292" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A293" s="3">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="B293" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A294" s="3">
+        <v>7.9861111111111105E-3</v>
+      </c>
+      <c r="B294" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A295" s="3">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="B295" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A296" s="3">
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="B296" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A297" s="3">
+        <v>2.2222222222222223E-2</v>
+      </c>
+      <c r="B297" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A298" s="3">
+        <v>2.2569444444444444E-2</v>
+      </c>
+      <c r="B298" s="2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A299" s="3">
+        <v>2.3958333333333335E-2</v>
+      </c>
+      <c r="B299" s="2" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A300" s="3">
+        <v>2.5694444444444443E-2</v>
+      </c>
+      <c r="B300" s="2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A301" s="3">
+        <v>2.9513888888888888E-2</v>
+      </c>
+      <c r="B301" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A302" s="3">
+        <v>3.4027777777777775E-2</v>
+      </c>
+      <c r="B302" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C302" s="2" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A303" s="3">
+        <v>3.8194444444444448E-2</v>
+      </c>
+      <c r="B303" s="2" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A304" s="3">
+        <v>3.9930555555555552E-2</v>
+      </c>
+      <c r="B304" s="2" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A305" s="3">
+        <v>4.0972222222222222E-2</v>
+      </c>
+      <c r="B305" s="2" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A306" s="3">
+        <v>4.3055555555555555E-2</v>
+      </c>
+      <c r="B306" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A307" s="3">
+        <v>4.6527777777777779E-2</v>
+      </c>
+      <c r="B307" s="2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A308" s="3">
+        <v>5.3819444444444448E-2</v>
+      </c>
+      <c r="B308" s="2" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A309" s="3">
+        <v>5.6944444444444443E-2</v>
+      </c>
+      <c r="B309" s="2" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A310" s="3">
+        <v>5.9722222222222225E-2</v>
+      </c>
+      <c r="B310" s="2" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A311" s="3">
+        <v>6.805555555555555E-2</v>
+      </c>
+      <c r="B311" s="2" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A312" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="B312" s="1" t="s">
+        <v>326</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hasta clase 16, Mango Avanzado (parte I)
</commit_message>
<xml_diff>
--- a/00-indice-videos.xlsx
+++ b/00-indice-videos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caryces\Desktop\CENDEZ\Formacion Academica\Programacion\Programacion Autonomo\coderhouse\04-Backend\01-info\Backend-I\_00-videos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{157B7D57-374B-4503-A8AB-1C3902416355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B898447A-2BE7-402F-B78A-0C6EDB7C7380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43200" yWindow="0" windowWidth="14400" windowHeight="15750" xr2:uid="{5152FF14-2E32-4855-8483-EEC7775E3DF9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="371">
   <si>
     <t>Clase 00</t>
   </si>
@@ -731,9 +731,6 @@
     <t>comando db.nombrecoleccion.insertOne({ propiedad1: "valor1", propiedad2: "valor2"})  ==&gt; crear un registro</t>
   </si>
   <si>
-    <t>comando db.nombrecoleccion.find()  ==&gt;  metodo para que devuelva todo lo que hay dentor de la colección</t>
-  </si>
-  <si>
     <t>El id se genera de forma automatica</t>
   </si>
   <si>
@@ -1017,6 +1014,141 @@
   </si>
   <si>
     <t>Primera práctica integradora</t>
+  </si>
+  <si>
+    <t>DAO ==&gt; Data Access Object (capa de abstraccion de acceso a los datos, separando de la logica del negocio)</t>
+  </si>
+  <si>
+    <t>Base de proyecto para la clase</t>
+  </si>
+  <si>
+    <t>product.dao.js de filesystem</t>
+  </si>
+  <si>
+    <t>connection.js de mongodb</t>
+  </si>
+  <si>
+    <t>product.model.js de models mongodb</t>
+  </si>
+  <si>
+    <t>Finalidad de morgan</t>
+  </si>
+  <si>
+    <t>errorHandler.js de middlewares</t>
+  </si>
+  <si>
+    <t>product.dao.js de mongodb</t>
+  </si>
+  <si>
+    <t>product.services.js de services</t>
+  </si>
+  <si>
+    <t>Comparacion de metodos de FS y mongo para los DAOs</t>
+  </si>
+  <si>
+    <t>products.controllers.js de controllers</t>
+  </si>
+  <si>
+    <t>product.router.js de routes</t>
+  </si>
+  <si>
+    <t>npm start y correccion de errores</t>
+  </si>
+  <si>
+    <t>prueba con postman</t>
+  </si>
+  <si>
+    <t>comando db.nombrecoleccion.find()  ==&gt;  metodo para que devuelva todo lo que hay dentro de la colección</t>
+  </si>
+  <si>
+    <t>Cambiando de Persistencia, de Mongo a FS</t>
+  </si>
+  <si>
+    <t>Repaso de lo hecho en clase</t>
+  </si>
+  <si>
+    <t>Clase 16</t>
+  </si>
+  <si>
+    <t>Mongo Avanzado (Parte I)</t>
+  </si>
+  <si>
+    <t>https://mongoosejs.com</t>
+  </si>
+  <si>
+    <t>Indexacion</t>
+  </si>
+  <si>
+    <t>Con indexacion se puede hacer la busqueda mas rapido porque ya se tiene la informaicon segmentada.</t>
+  </si>
+  <si>
+    <t>Por defecto una busqueda por ID ya esta indexada, por eso es más rápida</t>
+  </si>
+  <si>
+    <t>Ejemplo usando un JSON con 5000 usuarios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">npm i dotenv </t>
+  </si>
+  <si>
+    <t>Variables de entorno .env Se trabajan por key ==&gt; value</t>
+  </si>
+  <si>
+    <t>Subiendo los 5000 usuarios a la base de daots mongo Atlas</t>
+  </si>
+  <si>
+    <t>Agregando metodo para buscar por nombre sin indexacion, en esos 5000 usuarios</t>
+  </si>
+  <si>
+    <t>Metodo explain() de mongoose para ver todoa la informacion de la consulta</t>
+  </si>
+  <si>
+    <t>en el Mongo Compass se pueden ver los campos indexados</t>
+  </si>
+  <si>
+    <t>Como se indexa? Se agrega la propiedad index: true</t>
+  </si>
+  <si>
+    <t>Population en mongoose</t>
+  </si>
+  <si>
+    <t>Populations - Referenciar id de otros regustros en uno, ej, los id de mascotas de un usuario</t>
+  </si>
+  <si>
+    <t>En el modelo del usuario se guarda el array de mascotas del usuario</t>
+  </si>
+  <si>
+    <t>{ type: Schema.Types.ObjectId, ref: "pets", default: [] }</t>
+  </si>
+  <si>
+    <t>addPetToUser para agregar una mascota al usuario</t>
+  </si>
+  <si>
+    <t>agregando a user.services el addPetToUser</t>
+  </si>
+  <si>
+    <t>agregando a user.controllers el addPetToUser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">agregando la ruta a users.router </t>
+  </si>
+  <si>
+    <t>realizando la prueba para agragar la mascota al usuario</t>
+  </si>
+  <si>
+    <t>agregando el metodo populate para ver la informacion completa de la mascota en el usuario, no solo el id</t>
+  </si>
+  <si>
+    <t>Internamente mongoose busca los datos en la colección de la mascota para visualizarlos</t>
+  </si>
+  <si>
+    <t>middleware para agregar el populate User.Schema.pre('find', function(){this.populate('pets')})</t>
+  </si>
+  <si>
+    <t>Clase 17</t>
+  </si>
+  <si>
+    <t>Mongo Avanzado (Parte II)</t>
   </si>
 </sst>
 </file>
@@ -1429,10 +1561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8F680E1-5CBF-4782-AF11-5D549B1A7385}">
-  <dimension ref="A1:C312"/>
+  <dimension ref="A1:C354"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A280" workbookViewId="0">
-      <selection activeCell="A313" sqref="A313"/>
+    <sheetView tabSelected="1" topLeftCell="A326" workbookViewId="0">
+      <selection activeCell="B354" sqref="B354"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1447,7 +1579,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1503,7 +1635,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -1615,7 +1747,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -1687,7 +1819,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -1799,7 +1931,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -1959,7 +2091,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
@@ -2167,7 +2299,7 @@
         <v>90</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
@@ -2343,7 +2475,7 @@
         <v>112</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
@@ -2503,7 +2635,7 @@
         <v>132</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
@@ -2663,7 +2795,7 @@
         <v>151</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
@@ -2799,7 +2931,7 @@
         <v>184</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.2">
@@ -2951,7 +3083,7 @@
         <v>186</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.2">
@@ -3127,7 +3259,7 @@
         <v>209</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.2">
@@ -3295,7 +3427,7 @@
         <v>5.6250000000000001E-2</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>231</v>
+        <v>340</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.2">
@@ -3311,7 +3443,7 @@
         <v>5.7638888888888892E-2</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.2">
@@ -3319,7 +3451,7 @@
         <v>6.0416666666666667E-2</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.2">
@@ -3327,7 +3459,7 @@
         <v>6.1111111111111109E-2</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.2">
@@ -3335,7 +3467,7 @@
         <v>6.1805555555555558E-2</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.2">
@@ -3343,7 +3475,7 @@
         <v>6.2847222222222221E-2</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.2">
@@ -3351,7 +3483,7 @@
         <v>6.3541666666666663E-2</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.2">
@@ -3359,7 +3491,7 @@
         <v>6.458333333333334E-2</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.2">
@@ -3367,7 +3499,7 @@
         <v>6.5625000000000003E-2</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.2">
@@ -3375,7 +3507,7 @@
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.2">
@@ -3383,15 +3515,15 @@
         <v>6.7013888888888887E-2</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A244" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.2">
@@ -3399,7 +3531,7 @@
         <v>3.1250000000000002E-3</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.2">
@@ -3407,7 +3539,7 @@
         <v>5.208333333333333E-3</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.2">
@@ -3415,7 +3547,7 @@
         <v>9.3749999999999997E-3</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.2">
@@ -3431,7 +3563,7 @@
         <v>1.1111111111111112E-2</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.2">
@@ -3439,7 +3571,7 @@
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.2">
@@ -3447,7 +3579,7 @@
         <v>1.3194444444444444E-2</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.2">
@@ -3455,7 +3587,7 @@
         <v>1.4583333333333334E-2</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.2">
@@ -3463,7 +3595,7 @@
         <v>1.7708333333333333E-2</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.2">
@@ -3471,7 +3603,7 @@
         <v>1.8749999999999999E-2</v>
       </c>
       <c r="B254" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.2">
@@ -3479,7 +3611,7 @@
         <v>2.1874999999999999E-2</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.2">
@@ -3487,7 +3619,7 @@
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.2">
@@ -3495,7 +3627,7 @@
         <v>2.6388888888888889E-2</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.2">
@@ -3503,7 +3635,7 @@
         <v>2.9166666666666667E-2</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.2">
@@ -3511,7 +3643,7 @@
         <v>2.9513888888888888E-2</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.2">
@@ -3519,7 +3651,7 @@
         <v>2.9861111111111113E-2</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.2">
@@ -3527,7 +3659,7 @@
         <v>3.0902777777777779E-2</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.2">
@@ -3535,7 +3667,7 @@
         <v>3.125E-2</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.2">
@@ -3543,7 +3675,7 @@
         <v>3.2638888888888891E-2</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.2">
@@ -3551,7 +3683,7 @@
         <v>3.3680555555555554E-2</v>
       </c>
       <c r="B264" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.2">
@@ -3559,7 +3691,7 @@
         <v>3.4722222222222224E-2</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.2">
@@ -3567,7 +3699,7 @@
         <v>3.5763888888888887E-2</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.2">
@@ -3575,7 +3707,7 @@
         <v>3.6111111111111108E-2</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.2">
@@ -3583,7 +3715,7 @@
         <v>3.6458333333333336E-2</v>
       </c>
       <c r="B268" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.2">
@@ -3591,7 +3723,7 @@
         <v>4.6527777777777779E-2</v>
       </c>
       <c r="B269" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.2">
@@ -3599,7 +3731,7 @@
         <v>4.791666666666667E-2</v>
       </c>
       <c r="B270" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.2">
@@ -3607,7 +3739,7 @@
         <v>4.8611111111111112E-2</v>
       </c>
       <c r="B271" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.2">
@@ -3615,7 +3747,7 @@
         <v>5.2777777777777778E-2</v>
       </c>
       <c r="B272" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.2">
@@ -3623,7 +3755,7 @@
         <v>5.5208333333333331E-2</v>
       </c>
       <c r="B273" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.2">
@@ -3631,7 +3763,7 @@
         <v>5.6250000000000001E-2</v>
       </c>
       <c r="B274" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.2">
@@ -3639,7 +3771,7 @@
         <v>5.6944444444444443E-2</v>
       </c>
       <c r="B275" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.2">
@@ -3647,7 +3779,7 @@
         <v>5.7291666666666664E-2</v>
       </c>
       <c r="B276" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.2">
@@ -3655,7 +3787,7 @@
         <v>5.8680555555555555E-2</v>
       </c>
       <c r="B277" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.2">
@@ -3663,7 +3795,7 @@
         <v>6.2152777777777779E-2</v>
       </c>
       <c r="B278" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.2">
@@ -3671,7 +3803,7 @@
         <v>6.4236111111111105E-2</v>
       </c>
       <c r="B279" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.2">
@@ -3679,7 +3811,7 @@
         <v>6.805555555555555E-2</v>
       </c>
       <c r="B280" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.2">
@@ -3687,7 +3819,7 @@
         <v>6.9791666666666669E-2</v>
       </c>
       <c r="B281" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.2">
@@ -3695,7 +3827,7 @@
         <v>7.256944444444445E-2</v>
       </c>
       <c r="B282" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.2">
@@ -3703,7 +3835,7 @@
         <v>7.4305555555555555E-2</v>
       </c>
       <c r="B283" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.2">
@@ -3711,7 +3843,7 @@
         <v>7.4652777777777776E-2</v>
       </c>
       <c r="B284" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.2">
@@ -3719,7 +3851,7 @@
         <v>7.5694444444444439E-2</v>
       </c>
       <c r="B285" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.2">
@@ -3727,7 +3859,7 @@
         <v>7.7083333333333337E-2</v>
       </c>
       <c r="B286" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.2">
@@ -3735,15 +3867,15 @@
         <v>7.7430555555555558E-2</v>
       </c>
       <c r="B287" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A288" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.2">
@@ -3751,7 +3883,7 @@
         <v>2.4305555555555556E-3</v>
       </c>
       <c r="B289" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.2">
@@ -3759,7 +3891,7 @@
         <v>3.1250000000000002E-3</v>
       </c>
       <c r="B290" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.2">
@@ -3767,7 +3899,7 @@
         <v>3.472222222222222E-3</v>
       </c>
       <c r="B291" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.2">
@@ -3775,7 +3907,7 @@
         <v>4.8611111111111112E-3</v>
       </c>
       <c r="B292" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.2">
@@ -3783,7 +3915,7 @@
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="B293" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.2">
@@ -3791,7 +3923,7 @@
         <v>7.9861111111111105E-3</v>
       </c>
       <c r="B294" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.2">
@@ -3799,7 +3931,7 @@
         <v>1.5625E-2</v>
       </c>
       <c r="B295" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.2">
@@ -3807,7 +3939,7 @@
         <v>1.6666666666666666E-2</v>
       </c>
       <c r="B296" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.2">
@@ -3815,7 +3947,7 @@
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="B297" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.2">
@@ -3823,7 +3955,7 @@
         <v>2.2569444444444444E-2</v>
       </c>
       <c r="B298" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.2">
@@ -3831,7 +3963,7 @@
         <v>2.3958333333333335E-2</v>
       </c>
       <c r="B299" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.2">
@@ -3839,7 +3971,7 @@
         <v>2.5694444444444443E-2</v>
       </c>
       <c r="B300" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.2">
@@ -3847,7 +3979,7 @@
         <v>2.9513888888888888E-2</v>
       </c>
       <c r="B301" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.2">
@@ -3855,10 +3987,10 @@
         <v>3.4027777777777775E-2</v>
       </c>
       <c r="B302" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C302" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.2">
@@ -3866,7 +3998,7 @@
         <v>3.8194444444444448E-2</v>
       </c>
       <c r="B303" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.2">
@@ -3874,7 +4006,7 @@
         <v>3.9930555555555552E-2</v>
       </c>
       <c r="B304" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.2">
@@ -3882,7 +4014,7 @@
         <v>4.0972222222222222E-2</v>
       </c>
       <c r="B305" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.2">
@@ -3890,7 +4022,7 @@
         <v>4.3055555555555555E-2</v>
       </c>
       <c r="B306" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.2">
@@ -3898,7 +4030,7 @@
         <v>4.6527777777777779E-2</v>
       </c>
       <c r="B307" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.2">
@@ -3906,7 +4038,7 @@
         <v>5.3819444444444448E-2</v>
       </c>
       <c r="B308" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.2">
@@ -3914,7 +4046,7 @@
         <v>5.6944444444444443E-2</v>
       </c>
       <c r="B309" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.2">
@@ -3922,7 +4054,7 @@
         <v>5.9722222222222225E-2</v>
       </c>
       <c r="B310" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.2">
@@ -3930,15 +4062,351 @@
         <v>6.805555555555555E-2</v>
       </c>
       <c r="B311" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A312" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="B312" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="B312" s="1" t="s">
+    </row>
+    <row r="313" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A313" s="3">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="B313" s="2" t="s">
         <v>326</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A314" s="3">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="B314" s="2" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A315" s="3">
+        <v>7.6388888888888886E-3</v>
+      </c>
+      <c r="B315" s="2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A316" s="3">
+        <v>7.9861111111111105E-3</v>
+      </c>
+      <c r="B316" s="2" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A317" s="3">
+        <v>9.0277777777777769E-3</v>
+      </c>
+      <c r="B317" s="2" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A318" s="3">
+        <v>1.0069444444444445E-2</v>
+      </c>
+      <c r="B318" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A319" s="3">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="B319" s="2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A320" s="3">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="B320" s="5" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A321" s="3">
+        <v>1.8055555555555554E-2</v>
+      </c>
+      <c r="B321" s="2" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A322" s="3">
+        <v>2.2569444444444444E-2</v>
+      </c>
+      <c r="B322" s="2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A323" s="3">
+        <v>2.9513888888888888E-2</v>
+      </c>
+      <c r="B323" s="2" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A324" s="3">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="B324" s="2" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A325" s="3">
+        <v>1.2152777777777778E-2</v>
+      </c>
+      <c r="B325" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A326" s="3">
+        <v>5.486111111111111E-2</v>
+      </c>
+      <c r="B326" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A327" s="3">
+        <v>5.7638888888888892E-2</v>
+      </c>
+      <c r="B327" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A328" s="3">
+        <v>5.9722222222222225E-2</v>
+      </c>
+      <c r="B328" s="2" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A329" s="3">
+        <v>6.2847222222222221E-2</v>
+      </c>
+      <c r="B329" s="2" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A330" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="B330" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A331" s="3">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="B331" s="2" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A332" s="3">
+        <v>5.5555555555555558E-3</v>
+      </c>
+      <c r="B332" s="2" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A333" s="3">
+        <v>5.9027777777777776E-3</v>
+      </c>
+      <c r="B333" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A334" s="3">
+        <v>7.9861111111111105E-3</v>
+      </c>
+      <c r="B334" s="2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A335" s="3">
+        <v>1.2847222222222222E-2</v>
+      </c>
+      <c r="B335" s="2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A336" s="3">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="B336" s="2" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A337" s="3">
+        <v>1.8402777777777778E-2</v>
+      </c>
+      <c r="B337" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A338" s="3">
+        <v>1.9444444444444445E-2</v>
+      </c>
+      <c r="B338" s="2" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A339" s="3">
+        <v>2.013888888888889E-2</v>
+      </c>
+      <c r="B339" s="2" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A340" s="3">
+        <v>2.361111111111111E-2</v>
+      </c>
+      <c r="B340" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A341" s="3">
+        <v>2.6041666666666668E-2</v>
+      </c>
+      <c r="B341" s="2" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A342" s="3">
+        <v>4.6180555555555558E-2</v>
+      </c>
+      <c r="B342" s="2" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A343" s="3">
+        <v>4.9305555555555554E-2</v>
+      </c>
+      <c r="B343" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A344" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="B344" s="2" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A345" s="3">
+        <v>5.0694444444444445E-2</v>
+      </c>
+      <c r="B345" s="2" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A346" s="3">
+        <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="B346" s="2" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A347" s="3">
+        <v>5.7291666666666664E-2</v>
+      </c>
+      <c r="B347" s="2" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A348" s="3">
+        <v>6.0763888888888888E-2</v>
+      </c>
+      <c r="B348" s="2" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A349" s="3">
+        <v>6.3194444444444442E-2</v>
+      </c>
+      <c r="B349" s="2" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A350" s="3">
+        <v>6.4236111111111105E-2</v>
+      </c>
+      <c r="B350" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A351" s="3">
+        <v>6.5972222222222224E-2</v>
+      </c>
+      <c r="B351" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A352" s="3">
+        <v>6.7361111111111108E-2</v>
+      </c>
+      <c r="B352" s="2" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A353" s="3">
+        <v>6.8750000000000006E-2</v>
+      </c>
+      <c r="B353" s="2" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A354" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="B354" s="1" t="s">
+        <v>370</v>
       </c>
     </row>
   </sheetData>
@@ -3950,6 +4418,7 @@
     <hyperlink ref="B159" r:id="rId5" xr:uid="{4D4E83DE-12E0-4CC4-A2AF-BAF0D713C890}"/>
     <hyperlink ref="B220" r:id="rId6" xr:uid="{E64B71A3-0A70-4B59-8BFF-91A511B7C9DF}"/>
     <hyperlink ref="B222" r:id="rId7" xr:uid="{F9522E13-F5EE-4FBD-8D24-BB6E6916396D}"/>
+    <hyperlink ref="B320" r:id="rId8" xr:uid="{32CD77E5-DD2C-4087-9AEA-525BCF246A54}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>